<commit_message>
Add world and excel files
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self Learn\Frontend\Group\Diner\Task Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA894DA-B9C5-43BC-AE9D-A5CE51B30F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B4271A-4C8B-4B92-8172-27A68C66A764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -63,33 +63,12 @@
     <t>Header</t>
   </si>
   <si>
-    <t>Dev1</t>
-  </si>
-  <si>
     <t>Dev2</t>
   </si>
   <si>
-    <t xml:space="preserve">     Logo</t>
-  </si>
-  <si>
-    <t>Dev A</t>
-  </si>
-  <si>
     <t>Nhật Trường</t>
   </si>
   <si>
-    <t xml:space="preserve">   Navbar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Submenu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Search form</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Login popup</t>
-  </si>
-  <si>
     <t>Carousel</t>
   </si>
   <si>
@@ -118,6 +97,69 @@
   </si>
   <si>
     <t xml:space="preserve">Footer </t>
+  </si>
+  <si>
+    <t>Viết file tổng hợp + phân chia công việc</t>
+  </si>
+  <si>
+    <t>Ánh Ngọc</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Nguyên Phi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark theme </t>
+  </si>
+  <si>
+    <t>Search form</t>
+  </si>
+  <si>
+    <t>Submenu</t>
+  </si>
+  <si>
+    <t>Navbar</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Image (Left)</t>
+  </si>
+  <si>
+    <t>Content (right)</t>
+  </si>
+  <si>
+    <t>Grid Layout</t>
+  </si>
+  <si>
+    <t>Hover</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Back to top</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Form</t>
   </si>
 </sst>
 </file>
@@ -127,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,11 +198,6 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -203,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -322,14 +359,29 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -355,9 +407,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -365,17 +414,8 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,23 +424,132 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -637,19 +786,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J986"/>
+  <dimension ref="A2:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="2" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" customWidth="1"/>
     <col min="6" max="6" width="12.08203125" customWidth="1"/>
     <col min="7" max="7" width="10.75" customWidth="1"/>
     <col min="8" max="8" width="12.08203125" customWidth="1"/>
@@ -658,324 +806,631 @@
     <col min="11" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="37" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="22">
+        <v>37163</v>
+      </c>
+      <c r="C3" s="22">
+        <v>44469</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="11">
-        <v>0.95</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="16">
-        <f>SUM(D5:D7)/3</f>
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>13</v>
+      <c r="C4" s="8"/>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="17">
-        <f>SUM(H5:H7)/3</f>
+      <c r="H4" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="13">
+        <f>SUM(H7:H9)/3</f>
         <v>0.9</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="16">
+      <c r="I6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+      <c r="A7" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="17">
-        <v>1</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="16">
+      <c r="I7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+      <c r="A8" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="13">
         <v>0.9</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="17">
-        <v>0.9</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="16">
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+      <c r="A9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="13">
         <v>0.8</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="11">
-        <v>1</v>
-      </c>
-      <c r="I8" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>22</v>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="6" t="s">
-        <v>23</v>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
+    </row>
+    <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="11"/>
+    </row>
+    <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="11"/>
+    </row>
+    <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="11"/>
+    </row>
+    <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="10">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1914,14 +2369,49 @@
     <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="D2 D4:D14">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="H6:H24">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2 H4:H14">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D34">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H33">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "Update sub task"
This reverts commit 87620526863d11b6a333aa9c6fe7b4aa7a88349b.
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0263BDA-5311-401E-B07C-EC3ECE341E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B4271A-4C8B-4B92-8172-27A68C66A764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -117,6 +117,12 @@
     <t>Search form</t>
   </si>
   <si>
+    <t>Submenu</t>
+  </si>
+  <si>
+    <t>Navbar</t>
+  </si>
+  <si>
     <t>Logo</t>
   </si>
   <si>
@@ -154,15 +160,6 @@
   </si>
   <si>
     <t>Form</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Nav</t>
-  </si>
-  <si>
-    <t>Responsive</t>
   </si>
 </sst>
 </file>
@@ -384,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -406,6 +403,9 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -457,248 +457,11 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1023,10 +786,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:J1016"/>
+  <dimension ref="A2:J1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1071,868 +834,619 @@
       <c r="I2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="22">
         <v>37163</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="22">
         <v>44469</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="23">
         <v>1</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="20"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C4" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="9">
+      <c r="H4" s="10">
         <v>0.95</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="11"/>
     </row>
     <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C5" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8"/>
+      <c r="A5" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="11">
+      <c r="H5" s="12">
         <v>0.5</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="11"/>
     </row>
     <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C6" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D6" s="9">
-        <v>1</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="A6" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="12">
+      <c r="H6" s="13">
         <f>SUM(H7:H9)/3</f>
         <v>0.9</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A7" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C7" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D7" s="9">
+      <c r="A7" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="13">
         <v>1</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="12">
+      <c r="I7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+      <c r="A8" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+      <c r="A9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="10">
         <v>1</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A8" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C8" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="27">
-        <v>44470</v>
-      </c>
-      <c r="C9" s="27">
-        <v>44470</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>12</v>
+      <c r="A11" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="9">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="9">
-        <v>1</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
-        <v>29</v>
+      <c r="A12" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8"/>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
-        <v>30</v>
+      <c r="A13" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="9">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8"/>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
-        <v>43</v>
+      <c r="A14" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-      <c r="E14" s="8"/>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>13</v>
+      <c r="A15" s="24" t="s">
+        <v>33</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="23" t="s">
-        <v>29</v>
+      <c r="A16" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="23" t="s">
-        <v>43</v>
+      <c r="A17" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8"/>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>14</v>
+      <c r="A18" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="9">
-        <v>0</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="23" t="s">
-        <v>31</v>
+      <c r="A19" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8"/>
+      <c r="D19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
-        <v>32</v>
+      <c r="A20" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8"/>
+      <c r="D20" s="10">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="23" t="s">
-        <v>43</v>
+      <c r="A21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="9">
-        <v>0</v>
-      </c>
-      <c r="E21" s="8"/>
+      <c r="D21" s="10">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="6" t="s">
-        <v>15</v>
+      <c r="A22" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="D22" s="10">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="23" t="s">
-        <v>33</v>
+      <c r="A23" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8"/>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="23" t="s">
-        <v>34</v>
+      <c r="A24" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8"/>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="23" t="s">
-        <v>43</v>
+      <c r="A25" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-      <c r="E25" s="8"/>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>25</v>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="23" t="s">
-        <v>29</v>
+      <c r="A27" s="24" t="s">
+        <v>38</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-      <c r="E27" s="8"/>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="23" t="s">
-        <v>43</v>
+      <c r="A28" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="8"/>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>23</v>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="23" t="s">
-        <v>35</v>
+      <c r="A30" s="25" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-      <c r="E30" s="8"/>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="23" t="s">
-        <v>17</v>
+      <c r="A31" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-      <c r="E31" s="8"/>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="23" t="s">
-        <v>43</v>
+      <c r="A32" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-      <c r="E32" s="8"/>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="9">
-        <v>0</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="23" t="s">
-        <v>29</v>
+      <c r="A34" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="9">
-        <v>0</v>
-      </c>
-      <c r="E34" s="8"/>
+      <c r="D34" s="10">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="10"/>
-    </row>
-    <row r="35" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="9">
-        <v>0</v>
-      </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="10"/>
-    </row>
-    <row r="38" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="10"/>
-    </row>
-    <row r="39" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="10"/>
-    </row>
-    <row r="40" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="9">
-        <v>0</v>
-      </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="10"/>
-    </row>
-    <row r="41" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-      <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="10"/>
-    </row>
-    <row r="42" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="10"/>
-    </row>
-    <row r="43" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="10"/>
-    </row>
-    <row r="44" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="9">
-        <v>0</v>
-      </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="10"/>
-    </row>
-    <row r="45" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="9">
-        <v>0</v>
-      </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="10"/>
-    </row>
-    <row r="46" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="9">
-        <v>0</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="10"/>
-    </row>
-    <row r="47" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="9">
-        <v>0</v>
-      </c>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="10"/>
-    </row>
-    <row r="48" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="9">
-        <v>0</v>
-      </c>
-      <c r="E48" s="8"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="10"/>
-    </row>
-    <row r="49" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="9">
-        <v>0</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="10"/>
-    </row>
-    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2870,109 +2384,34 @@
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="greaterThan">
+  <conditionalFormatting sqref="H6:H24">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36 H39:H41 H43:H47">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="greaterThan">
+  <conditionalFormatting sqref="D5:D34">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="greaterThan">
+  <conditionalFormatting sqref="H25:H33">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Edit task Booking restaurant
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0263BDA-5311-401E-B07C-EC3ECE341E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687F5EC4-6590-4C16-8126-4EF1AA5B484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,150 +467,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1025,8 +882,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1109,12 +966,10 @@
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="26">
         <v>44470</v>
       </c>
-      <c r="C4" s="27">
-        <v>44470</v>
-      </c>
+      <c r="C4" s="27"/>
       <c r="D4" s="9">
         <v>0.8</v>
       </c>
@@ -1392,10 +1247,12 @@
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="26">
+        <v>44471</v>
+      </c>
       <c r="C18" s="7"/>
       <c r="D18" s="9">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>23</v>
@@ -1410,10 +1267,14 @@
       <c r="A19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="27">
+        <v>44471</v>
+      </c>
+      <c r="C19" s="27">
+        <v>44471</v>
+      </c>
       <c r="D19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="7"/>
@@ -1426,10 +1287,14 @@
       <c r="A20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="27">
+        <v>44471</v>
+      </c>
+      <c r="C20" s="27">
+        <v>44471</v>
+      </c>
       <c r="D20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="7"/>
@@ -2887,87 +2752,87 @@
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
-    <cfRule type="cellIs" dxfId="30" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="34" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="35" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36 H39:H41 H43:H47">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="26" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="31" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="21" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
xay dung xong carousel chưa test responsive
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Front End\BTVN\Dinner\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687F5EC4-6590-4C16-8126-4EF1AA5B484D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22776" windowHeight="14664"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mitsg4nKYzU0T1mG+CZd0js0eHfeQ=="/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -168,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -876,31 +875,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08203125" customWidth="1"/>
-    <col min="6" max="6" width="12.08203125" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="12.08203125" customWidth="1"/>
-    <col min="9" max="9" width="11.9140625" customWidth="1"/>
+    <col min="1" max="1" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" customWidth="1"/>
+    <col min="6" max="6" width="12.09765625" customWidth="1"/>
+    <col min="7" max="7" width="10.69921875" customWidth="1"/>
+    <col min="8" max="8" width="12.09765625" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="26" width="7.6640625" customWidth="1"/>
+    <col min="11" max="26" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,7 +931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>22</v>
       </c>
@@ -962,7 +961,7 @@
       </c>
       <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -986,7 +985,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>28</v>
       </c>
@@ -1010,7 +1009,7 @@
       </c>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
         <v>41</v>
       </c>
@@ -1035,7 +1034,7 @@
       </c>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>42</v>
       </c>
@@ -1059,7 +1058,7 @@
       </c>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>27</v>
       </c>
@@ -1083,7 +1082,7 @@
       </c>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>26</v>
       </c>
@@ -1107,7 +1106,7 @@
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>43</v>
       </c>
@@ -1123,14 +1122,14 @@
       <c r="I10" s="8"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>25</v>
@@ -1138,46 +1137,62 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="27">
+        <v>44470</v>
+      </c>
+      <c r="C12" s="27">
+        <v>44470</v>
+      </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="8"/>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="27">
+        <v>44470</v>
+      </c>
+      <c r="C13" s="27">
+        <v>44470</v>
+      </c>
       <c r="D13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="8"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23" t="s">
         <v>43</v>
       </c>
@@ -1193,7 +1208,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -1211,7 +1226,7 @@
       <c r="I15" s="8"/>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23" t="s">
         <v>29</v>
       </c>
@@ -1227,7 +1242,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="23" t="s">
         <v>43</v>
       </c>
@@ -1243,7 +1258,7 @@
       <c r="I17" s="8"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
@@ -1263,7 +1278,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
         <v>31</v>
       </c>
@@ -1283,7 +1298,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1318,7 @@
       <c r="I20" s="8"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>43</v>
       </c>
@@ -1319,7 +1334,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>15</v>
       </c>
@@ -1337,7 +1352,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="23" t="s">
         <v>33</v>
       </c>
@@ -1353,7 +1368,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="23" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1384,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="23" t="s">
         <v>43</v>
       </c>
@@ -1385,7 +1400,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>16</v>
       </c>
@@ -1403,7 +1418,7 @@
       <c r="I26" s="8"/>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1434,7 @@
       <c r="I27" s="8"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="23" t="s">
         <v>43</v>
       </c>
@@ -1435,7 +1450,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>17</v>
       </c>
@@ -1453,7 +1468,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="23" t="s">
         <v>35</v>
       </c>
@@ -1469,7 +1484,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="23" t="s">
         <v>17</v>
       </c>
@@ -1485,7 +1500,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="23" t="s">
         <v>43</v>
       </c>
@@ -1501,7 +1516,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>18</v>
       </c>
@@ -1519,7 +1534,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
         <v>29</v>
       </c>
@@ -1535,7 +1550,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>43</v>
       </c>
@@ -1551,7 +1566,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>19</v>
       </c>
@@ -1569,7 +1584,7 @@
       <c r="I36" s="8"/>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>29</v>
       </c>
@@ -1585,7 +1600,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23" t="s">
         <v>43</v>
       </c>
@@ -1601,7 +1616,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1634,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="23" t="s">
         <v>36</v>
       </c>
@@ -1635,7 +1650,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="23" t="s">
         <v>12</v>
       </c>
@@ -1651,7 +1666,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
         <v>43</v>
       </c>
@@ -1667,7 +1682,7 @@
       <c r="I42" s="8"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
@@ -1685,7 +1700,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="24" t="s">
         <v>38</v>
       </c>
@@ -1701,7 +1716,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="25" t="s">
         <v>33</v>
       </c>
@@ -1717,7 +1732,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="25" t="s">
         <v>40</v>
       </c>
@@ -1733,7 +1748,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="24" t="s">
         <v>39</v>
       </c>
@@ -1749,7 +1764,7 @@
       <c r="I47" s="8"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="23" t="s">
         <v>43</v>
       </c>
@@ -1765,7 +1780,7 @@
       <c r="I48" s="8"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>37</v>
       </c>
@@ -1783,973 +1798,973 @@
       <c r="I49" s="8"/>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
     <cfRule type="cellIs" dxfId="17" priority="34" operator="greaterThan">

</xml_diff>

<commit_message>
Add date for news task
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF3063-6B74-41CB-A698-7E988ECBA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67FEA3C-0E0E-44B7-9940-017130535393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,18 +461,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -887,8 +876,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1348,7 +1337,9 @@
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="26">
+        <v>44473</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="9">
         <v>0</v>
@@ -1366,8 +1357,12 @@
       <c r="A23" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="27">
+        <v>44473</v>
+      </c>
+      <c r="C23" s="27">
+        <v>44474</v>
+      </c>
       <c r="D23" s="9">
         <v>0</v>
       </c>
@@ -1382,7 +1377,9 @@
       <c r="A24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="27">
+        <v>44473</v>
+      </c>
       <c r="C24" s="7"/>
       <c r="D24" s="9">
         <v>0</v>
@@ -2777,92 +2774,92 @@
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
-    <cfRule type="cellIs" dxfId="18" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="34" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="17" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="35" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36 H39:H41 H43:H47">
-    <cfRule type="cellIs" dxfId="16" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="15" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="31" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="23" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="21" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D49">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revert "Add date for news task"
This reverts commit dbe3f1a09f849fcbddcfe3d668a7665616fb001a.
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67FEA3C-0E0E-44B7-9940-017130535393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF3063-6B74-41CB-A698-7E988ECBA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -876,8 +887,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1337,9 +1348,7 @@
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="26">
-        <v>44473</v>
-      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="9">
         <v>0</v>
@@ -1357,12 +1366,8 @@
       <c r="A23" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="27">
-        <v>44473</v>
-      </c>
-      <c r="C23" s="27">
-        <v>44474</v>
-      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="9">
         <v>0</v>
       </c>
@@ -1377,9 +1382,7 @@
       <c r="A24" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="27">
-        <v>44473</v>
-      </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="9">
         <v>0</v>
@@ -2774,92 +2777,92 @@
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
-    <cfRule type="cellIs" dxfId="17" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="34" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="16" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="35" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36 H39:H41 H43:H47">
-    <cfRule type="cellIs" dxfId="15" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="33" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="14" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="31" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="13" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="29" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="12" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="25" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="7" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add date for task
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF3063-6B74-41CB-A698-7E988ECBA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C74468-7D8C-4DF7-AA16-434E57BB6EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -408,10 +408,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -887,8 +883,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -933,48 +929,48 @@
       <c r="I2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="19">
         <v>37163</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="19">
         <v>44469</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="20">
         <v>1</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="20"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>44470</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="9">
         <v>0.8</v>
       </c>
@@ -987,13 +983,13 @@
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="25">
         <v>44470</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="25">
         <v>44470</v>
       </c>
       <c r="D5" s="9">
@@ -1002,18 +998,18 @@
       <c r="E5" s="8"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="11"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="8"/>
       <c r="J5" s="10"/>
     </row>
     <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="25">
         <v>44470</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="25">
         <v>44470</v>
       </c>
       <c r="D6" s="9">
@@ -1022,91 +1018,91 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="8"/>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="25">
         <v>44470</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <v>44470</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="8"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="25">
         <v>44470</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="25">
         <v>44470</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="8"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="25">
         <v>44470</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <v>44470</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="9">
         <v>0</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="13"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="9"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="24">
         <v>44471</v>
       </c>
       <c r="C11" s="7"/>
@@ -1116,7 +1112,7 @@
       <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="24">
         <v>44473</v>
       </c>
       <c r="G11" s="7"/>
@@ -1129,23 +1125,23 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="25">
         <v>44471</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="25">
         <v>44471</v>
       </c>
       <c r="D12" s="9">
         <v>1</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="27">
+      <c r="F12" s="25">
         <v>44473</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="25">
         <v>44474</v>
       </c>
       <c r="H12" s="9">
@@ -1155,23 +1151,23 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="25">
         <v>44471</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <v>44471</v>
       </c>
       <c r="D13" s="9">
         <v>1</v>
       </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <v>44473</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="25">
         <v>44474</v>
       </c>
       <c r="H13" s="9">
@@ -1181,7 +1177,7 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="7"/>
@@ -1200,7 +1196,7 @@
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="24">
         <v>44471</v>
       </c>
       <c r="C15" s="7"/>
@@ -1210,7 +1206,7 @@
       <c r="E15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="24">
         <v>44473</v>
       </c>
       <c r="G15" s="7"/>
@@ -1223,23 +1219,23 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="25">
         <v>44471</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="25">
         <v>44471</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
       <c r="E16" s="8"/>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>44473</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="25">
         <v>44474</v>
       </c>
       <c r="H16" s="9">
@@ -1249,7 +1245,7 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B17" s="7"/>
@@ -1258,12 +1254,8 @@
         <v>0</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="27">
-        <v>44473</v>
-      </c>
-      <c r="G17" s="27">
-        <v>44474</v>
-      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="9"/>
       <c r="I17" s="8"/>
       <c r="J17" s="10"/>
@@ -1272,7 +1264,7 @@
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="24">
         <v>44471</v>
       </c>
       <c r="C18" s="7"/>
@@ -1289,13 +1281,13 @@
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="25">
         <v>44471</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="25">
         <v>44471</v>
       </c>
       <c r="D19" s="9">
@@ -1309,13 +1301,13 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="25">
         <v>44471</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="25">
         <v>44471</v>
       </c>
       <c r="D20" s="9">
@@ -1329,7 +1321,7 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="7"/>
@@ -1348,10 +1340,12 @@
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="24">
+        <v>44473</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="9">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>21</v>
@@ -1363,13 +1357,17 @@
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
+      <c r="B23" s="25">
+        <v>44473</v>
+      </c>
+      <c r="C23" s="25">
+        <v>44474</v>
+      </c>
       <c r="D23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
@@ -1379,13 +1377,17 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="25">
+        <v>44473</v>
+      </c>
+      <c r="C24" s="25">
+        <v>44474</v>
+      </c>
       <c r="D24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="7"/>
@@ -1395,7 +1397,7 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="7"/>
@@ -1429,7 +1431,7 @@
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="7"/>
@@ -1445,7 +1447,7 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="7"/>
@@ -1479,7 +1481,7 @@
       <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="7"/>
@@ -1495,7 +1497,7 @@
       <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="7"/>
@@ -1511,7 +1513,7 @@
       <c r="J31" s="10"/>
     </row>
     <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B32" s="7"/>
@@ -1545,7 +1547,7 @@
       <c r="J33" s="10"/>
     </row>
     <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="7"/>
@@ -1561,7 +1563,7 @@
       <c r="J34" s="10"/>
     </row>
     <row r="35" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="7"/>
@@ -1595,7 +1597,7 @@
       <c r="J36" s="10"/>
     </row>
     <row r="37" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B37" s="7"/>
@@ -1611,7 +1613,7 @@
       <c r="J37" s="10"/>
     </row>
     <row r="38" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="7"/>
@@ -1645,7 +1647,7 @@
       <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="7"/>
@@ -1661,7 +1663,7 @@
       <c r="J40" s="10"/>
     </row>
     <row r="41" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B41" s="7"/>
@@ -1677,7 +1679,7 @@
       <c r="J41" s="10"/>
     </row>
     <row r="42" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B42" s="7"/>
@@ -1711,7 +1713,7 @@
       <c r="J43" s="10"/>
     </row>
     <row r="44" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B44" s="7"/>
@@ -1727,7 +1729,7 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B45" s="7"/>
@@ -1743,7 +1745,7 @@
       <c r="J45" s="10"/>
     </row>
     <row r="46" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="7"/>
@@ -1759,7 +1761,7 @@
       <c r="J46" s="10"/>
     </row>
     <row r="47" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B47" s="7"/>
@@ -1775,7 +1777,7 @@
       <c r="J47" s="10"/>
     </row>
     <row r="48" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B48" s="7"/>
@@ -2776,93 +2778,98 @@
     <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="H6:H16 H18:H20 H22:H24 H26 H29:H31 H33">
-    <cfRule type="cellIs" dxfId="18" priority="34" operator="greaterThan">
+  <conditionalFormatting sqref="H11:H16 H18:H20 H22:H24 H26 H29:H31 H33">
+    <cfRule type="cellIs" dxfId="18" priority="35" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="17" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="36" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36 H39:H41 H43:H47">
-    <cfRule type="cellIs" dxfId="16" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="34" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="15" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="32" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="14" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="30" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="26" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="14" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D49">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Create and do number section
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C74468-7D8C-4DF7-AA16-434E57BB6EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9D7595-DB29-464D-83C4-F6C7954D9011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1466,7 +1466,9 @@
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="24">
+        <v>44474</v>
+      </c>
       <c r="C29" s="7"/>
       <c r="D29" s="9">
         <v>0</v>
@@ -1484,7 +1486,9 @@
       <c r="A30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="25">
+        <v>44474</v>
+      </c>
       <c r="C30" s="7"/>
       <c r="D30" s="9">
         <v>0</v>

</xml_diff>

<commit_message>
Insert date for number section
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9D7595-DB29-464D-83C4-F6C7954D9011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE149138-2CAD-4989-AFB1-ACEDCE7BEFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="9">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>21</v>
@@ -1489,9 +1489,11 @@
       <c r="B30" s="25">
         <v>44474</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="25">
+        <v>44474</v>
+      </c>
       <c r="D30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="7"/>
@@ -1504,10 +1506,14 @@
       <c r="A31" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
+      <c r="B31" s="25">
+        <v>44474</v>
+      </c>
+      <c r="C31" s="25">
+        <v>44474</v>
+      </c>
       <c r="D31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="7"/>

</xml_diff>

<commit_message>
Create and done testimonial section
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE149138-2CAD-4989-AFB1-ACEDCE7BEFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75224B9F-0C9B-445A-939A-13AE065675CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1642,10 +1642,12 @@
       <c r="A39" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="7"/>
+      <c r="B39" s="24">
+        <v>44476</v>
+      </c>
       <c r="C39" s="7"/>
       <c r="D39" s="9">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>21</v>
@@ -1660,10 +1662,14 @@
       <c r="A40" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+      <c r="B40" s="25">
+        <v>44476</v>
+      </c>
+      <c r="C40" s="25">
+        <v>44476</v>
+      </c>
       <c r="D40" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="7"/>
@@ -1676,10 +1682,14 @@
       <c r="A41" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
+      <c r="B41" s="25">
+        <v>44476</v>
+      </c>
+      <c r="C41" s="25">
+        <v>44476</v>
+      </c>
       <c r="D41" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="7"/>

</xml_diff>

<commit_message>
Add date for responsive task (header and book section)
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Front End\BTVN\Dinner\Diner\Task Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E2D37D-BA0E-4FBA-A237-87D7D27F156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22776" windowHeight="14664"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -161,7 +162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -377,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -452,11 +453,23 @@
     <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1030,31 +1043,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.09765625" customWidth="1"/>
-    <col min="6" max="6" width="12.09765625" customWidth="1"/>
-    <col min="7" max="7" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.09765625" customWidth="1"/>
-    <col min="9" max="9" width="11.8984375" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" customWidth="1"/>
+    <col min="7" max="7" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08203125" customWidth="1"/>
+    <col min="9" max="9" width="11.9140625" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="26" width="7.69921875" customWidth="1"/>
+    <col min="11" max="26" width="7.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1086,7 +1099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1116,16 +1129,18 @@
       </c>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="24">
         <v>44470</v>
       </c>
-      <c r="C4" s="25"/>
+      <c r="C4" s="24">
+        <v>44480</v>
+      </c>
       <c r="D4" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>21</v>
@@ -1139,7 +1154,7 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
@@ -1161,7 +1176,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
         <v>39</v>
       </c>
@@ -1183,7 +1198,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A7" s="23" t="s">
         <v>40</v>
       </c>
@@ -1205,7 +1220,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A8" s="23" t="s">
         <v>25</v>
       </c>
@@ -1227,7 +1242,7 @@
       <c r="I8" s="8"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
@@ -1249,14 +1264,18 @@
       <c r="I9" s="8"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
       <c r="A10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="25">
+        <v>44480</v>
+      </c>
+      <c r="C10" s="25">
+        <v>44480</v>
+      </c>
       <c r="D10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="11"/>
@@ -1265,7 +1284,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -1291,7 +1310,7 @@
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
@@ -1317,7 +1336,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
@@ -1343,7 +1362,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="21" t="s">
         <v>41</v>
       </c>
@@ -1359,7 +1378,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1385,7 +1404,7 @@
       </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
@@ -1411,7 +1430,7 @@
       <c r="I16" s="8"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
         <v>41</v>
       </c>
@@ -1427,16 +1446,18 @@
       <c r="I17" s="8"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="24">
         <v>44471</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="24">
+        <v>44480</v>
+      </c>
       <c r="D18" s="9">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>21</v>
@@ -1447,7 +1468,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="21" t="s">
         <v>29</v>
       </c>
@@ -1467,7 +1488,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
@@ -1487,14 +1508,18 @@
       <c r="I20" s="8"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+      <c r="B21" s="25">
+        <v>44480</v>
+      </c>
+      <c r="C21" s="25">
+        <v>44480</v>
+      </c>
       <c r="D21" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="7"/>
@@ -1503,7 +1528,7 @@
       <c r="I21" s="8"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
@@ -1525,7 +1550,7 @@
       </c>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="21" t="s">
         <v>31</v>
       </c>
@@ -1547,7 +1572,7 @@
       <c r="I23" s="8"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="21" t="s">
         <v>32</v>
       </c>
@@ -1569,7 +1594,7 @@
       <c r="I24" s="8"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="21" t="s">
         <v>41</v>
       </c>
@@ -1585,7 +1610,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
@@ -1601,13 +1626,19 @@
       <c r="E26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="24">
+        <v>44478</v>
+      </c>
       <c r="G26" s="7"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="8"/>
+      <c r="H26" s="26">
+        <v>0.67</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
         <v>27</v>
       </c>
@@ -1621,13 +1652,19 @@
         <v>1</v>
       </c>
       <c r="E27" s="8"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="9"/>
+      <c r="F27" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G27" s="25">
+        <v>44478</v>
+      </c>
+      <c r="H27" s="26">
+        <v>1</v>
+      </c>
       <c r="I27" s="8"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
@@ -1643,7 +1680,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
@@ -1665,7 +1702,7 @@
       </c>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="21" t="s">
         <v>33</v>
       </c>
@@ -1687,7 +1724,7 @@
       <c r="I30" s="8"/>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
         <v>15</v>
       </c>
@@ -1709,7 +1746,7 @@
       <c r="I31" s="8"/>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="21" t="s">
         <v>41</v>
       </c>
@@ -1725,29 +1762,33 @@
       <c r="I32" s="8"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B33" s="24">
         <v>44474</v>
       </c>
-      <c r="C33" s="25">
-        <v>44477</v>
-      </c>
+      <c r="C33" s="25"/>
       <c r="D33" s="9">
         <v>0.6</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="24">
+        <v>44478</v>
+      </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8"/>
+      <c r="H33" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="21" t="s">
         <v>27</v>
       </c>
@@ -1761,13 +1802,19 @@
         <v>1</v>
       </c>
       <c r="E34" s="8"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="9"/>
+      <c r="F34" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G34" s="25">
+        <v>44478</v>
+      </c>
+      <c r="H34" s="26">
+        <v>1</v>
+      </c>
       <c r="I34" s="8"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
         <v>41</v>
       </c>
@@ -1783,29 +1830,33 @@
       <c r="I35" s="8"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="24">
         <v>44474</v>
       </c>
-      <c r="C36" s="25">
-        <v>44477</v>
-      </c>
+      <c r="C36" s="25"/>
       <c r="D36" s="9">
         <v>0.7</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="8"/>
+      <c r="F36" s="24">
+        <v>44478</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
         <v>27</v>
       </c>
@@ -1819,13 +1870,19 @@
         <v>1</v>
       </c>
       <c r="E37" s="8"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="9"/>
+      <c r="F37" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G37" s="25">
+        <v>44478</v>
+      </c>
+      <c r="H37" s="26">
+        <v>1</v>
+      </c>
       <c r="I37" s="8"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
         <v>41</v>
       </c>
@@ -1841,7 +1898,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>18</v>
       </c>
@@ -1863,7 +1920,7 @@
       </c>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
         <v>34</v>
       </c>
@@ -1885,7 +1942,7 @@
       <c r="I40" s="8"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
         <v>10</v>
       </c>
@@ -1907,7 +1964,7 @@
       <c r="I41" s="8"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
@@ -1923,29 +1980,33 @@
       <c r="I42" s="8"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="25">
+      <c r="B43" s="24">
         <v>44474</v>
       </c>
-      <c r="C43" s="25">
-        <v>44477</v>
-      </c>
+      <c r="C43" s="25"/>
       <c r="D43" s="9">
         <v>0.8</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="24">
+        <v>44478</v>
+      </c>
       <c r="G43" s="7"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="8"/>
+      <c r="H43" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="22" t="s">
         <v>36</v>
       </c>
@@ -1959,13 +2020,17 @@
         <v>1</v>
       </c>
       <c r="E44" s="8"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="9"/>
+      <c r="F44" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="26">
+        <v>0.8</v>
+      </c>
       <c r="I44" s="8"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="23" t="s">
         <v>31</v>
       </c>
@@ -1979,13 +2044,17 @@
         <v>1</v>
       </c>
       <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="9"/>
+      <c r="F45" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="26">
+        <v>0.8</v>
+      </c>
       <c r="I45" s="8"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="23" t="s">
         <v>38</v>
       </c>
@@ -1999,13 +2068,17 @@
         <v>1</v>
       </c>
       <c r="E46" s="8"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="9"/>
+      <c r="F46" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26">
+        <v>0.8</v>
+      </c>
       <c r="I46" s="8"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="22" t="s">
         <v>37</v>
       </c>
@@ -2019,13 +2092,17 @@
         <v>1</v>
       </c>
       <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="9"/>
+      <c r="F47" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G47" s="25"/>
+      <c r="H47" s="26">
+        <v>0.8</v>
+      </c>
       <c r="I47" s="8"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="21" t="s">
         <v>41</v>
       </c>
@@ -2037,18 +2114,18 @@
       <c r="E48" s="8"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="26"/>
       <c r="I48" s="8"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="25">
+      <c r="B49" s="24">
         <v>44477</v>
       </c>
-      <c r="C49" s="25">
+      <c r="C49" s="24">
         <v>44477</v>
       </c>
       <c r="D49" s="9">
@@ -2057,1126 +2134,1154 @@
       <c r="E49" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="8"/>
+      <c r="F49" s="24">
+        <v>44478</v>
+      </c>
+      <c r="G49" s="24">
+        <v>44478</v>
+      </c>
+      <c r="H49" s="26">
+        <v>1</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="H11:H16 H18:H20 H22 H26 H29 H33">
-    <cfRule type="cellIs" dxfId="32" priority="49" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36 H39 H43:H47">
-    <cfRule type="cellIs" dxfId="30" priority="48" operator="greaterThan">
+  <conditionalFormatting sqref="H11:H16 H18:H20 H22 H29">
+    <cfRule type="cellIs" dxfId="33" priority="58" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="cellIs" dxfId="32" priority="57" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="cellIs" dxfId="31" priority="53" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="cellIs" dxfId="30" priority="49" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="cellIs" dxfId="29" priority="47" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="cellIs" dxfId="28" priority="45" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="cellIs" dxfId="27" priority="41" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="cellIs" dxfId="26" priority="39" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38">
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D49">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:H47">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="29" priority="46" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="28" priority="44" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="27" priority="40" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="23" priority="32" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="cellIs" dxfId="21" priority="28" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="cellIs" dxfId="19" priority="24" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D49">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
+  <conditionalFormatting sqref="H36">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update date for reposive of news section
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E2D37D-BA0E-4FBA-A237-87D7D27F156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938AFCDF-54EF-463F-85DC-9C295069F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1535,9 +1535,11 @@
       <c r="B22" s="24">
         <v>44473</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="24">
+        <v>44481</v>
+      </c>
       <c r="D22" s="9">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>21</v>
@@ -1598,10 +1600,14 @@
       <c r="A25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="25">
+        <v>44481</v>
+      </c>
+      <c r="C25" s="25">
+        <v>44481</v>
+      </c>
       <c r="D25" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="7"/>

</xml_diff>

<commit_message>
Update date for number and testinomial section (responsive)
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938AFCDF-54EF-463F-85DC-9C295069F37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04513978-CA79-4A8A-B29E-A1BF9A04457A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1693,7 +1693,9 @@
       <c r="B29" s="24">
         <v>44474</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="24">
+        <v>44481</v>
+      </c>
       <c r="D29" s="9">
         <v>0.67</v>
       </c>
@@ -1756,8 +1758,12 @@
       <c r="A32" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="25">
+        <v>44481</v>
+      </c>
+      <c r="C32" s="25">
+        <v>44481</v>
+      </c>
       <c r="D32" s="9">
         <v>0</v>
       </c>
@@ -1911,7 +1917,9 @@
       <c r="B39" s="24">
         <v>44476</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="24">
+        <v>44481</v>
+      </c>
       <c r="D39" s="9">
         <v>0.67</v>
       </c>
@@ -1974,8 +1982,12 @@
       <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="B42" s="25">
+        <v>44481</v>
+      </c>
+      <c r="C42" s="25">
+        <v>44481</v>
+      </c>
       <c r="D42" s="9">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
update date for testing responsive
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04513978-CA79-4A8A-B29E-A1BF9A04457A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA1AA2E-E43C-49AF-B2A4-72E93CD4552F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,8 +1049,8 @@
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
@@ -1372,9 +1372,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="25">
+        <v>44482</v>
+      </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I14" s="8"/>
       <c r="J14" s="10"/>
     </row>
@@ -1440,9 +1444,13 @@
         <v>0</v>
       </c>
       <c r="E17" s="8"/>
-      <c r="F17" s="25"/>
+      <c r="F17" s="25">
+        <v>44482</v>
+      </c>
       <c r="G17" s="25"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="J17" s="10"/>
     </row>
@@ -1680,9 +1688,13 @@
         <v>0</v>
       </c>
       <c r="E28" s="8"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="25">
+        <v>44482</v>
+      </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="9"/>
+      <c r="H28" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I28" s="8"/>
       <c r="J28" s="10"/>
     </row>
@@ -1836,9 +1848,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
+      <c r="F35" s="25">
+        <v>44482</v>
+      </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I35" s="8"/>
       <c r="J35" s="10"/>
     </row>
@@ -1904,9 +1920,13 @@
         <v>0</v>
       </c>
       <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
+      <c r="F38" s="25">
+        <v>44482</v>
+      </c>
       <c r="G38" s="7"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9">
+        <v>0.8</v>
+      </c>
       <c r="I38" s="8"/>
       <c r="J38" s="10"/>
     </row>
@@ -2041,9 +2061,11 @@
       <c r="F44" s="25">
         <v>44478</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="25">
+        <v>44482</v>
+      </c>
       <c r="H44" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="10"/>
@@ -2065,9 +2087,11 @@
       <c r="F45" s="25">
         <v>44478</v>
       </c>
-      <c r="G45" s="25"/>
+      <c r="G45" s="25">
+        <v>44482</v>
+      </c>
       <c r="H45" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I45" s="8"/>
       <c r="J45" s="10"/>
@@ -2089,9 +2113,11 @@
       <c r="F46" s="25">
         <v>44478</v>
       </c>
-      <c r="G46" s="25"/>
+      <c r="G46" s="25">
+        <v>44482</v>
+      </c>
       <c r="H46" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="10"/>
@@ -2113,9 +2139,11 @@
       <c r="F47" s="25">
         <v>44478</v>
       </c>
-      <c r="G47" s="25"/>
+      <c r="G47" s="25">
+        <v>44482</v>
+      </c>
       <c r="H47" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I47" s="8"/>
       <c r="J47" s="10"/>
@@ -2130,9 +2158,13 @@
         <v>0</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="26"/>
+      <c r="F48" s="25">
+        <v>44482</v>
+      </c>
+      <c r="G48" s="25"/>
+      <c r="H48" s="26">
+        <v>0.8</v>
+      </c>
       <c r="I48" s="8"/>
       <c r="J48" s="10"/>
     </row>

</xml_diff>

<commit_message>
bổ sung template task
</commit_message>
<xml_diff>
--- a/Task Template/template_task.xlsx
+++ b/Task Template/template_task.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontend\HW\Diner\Task Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Front End\BTVN\Dinner\Diner\Task Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA1AA2E-E43C-49AF-B2A4-72E93CD4552F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22776" windowHeight="14664"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="43">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -157,12 +156,15 @@
   </si>
   <si>
     <t>Responsive</t>
+  </si>
+  <si>
+    <t>14/10/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -458,7 +460,62 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1043,31 +1100,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A2:J1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08203125" customWidth="1"/>
-    <col min="6" max="6" width="12.08203125" customWidth="1"/>
-    <col min="7" max="7" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08203125" customWidth="1"/>
-    <col min="9" max="9" width="11.9140625" customWidth="1"/>
+    <col min="1" max="1" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.19921875" customWidth="1"/>
+    <col min="4" max="4" width="7.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.09765625" customWidth="1"/>
+    <col min="6" max="6" width="12.09765625" customWidth="1"/>
+    <col min="7" max="7" width="13.59765625" customWidth="1"/>
+    <col min="8" max="8" width="12.09765625" customWidth="1"/>
+    <col min="9" max="9" width="11.8984375" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="26" width="7.6640625" customWidth="1"/>
+    <col min="11" max="26" width="7.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
@@ -1129,7 +1187,7 @@
       </c>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1145,16 +1203,21 @@
       <c r="E4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="F4" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G4" s="25">
+        <v>44473</v>
+      </c>
       <c r="H4" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>26</v>
       </c>
@@ -1168,15 +1231,19 @@
         <v>1</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G5" s="25">
+        <v>44473</v>
+      </c>
       <c r="H5" s="9">
         <v>1</v>
       </c>
       <c r="I5" s="8"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="44" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="43.95" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>39</v>
       </c>
@@ -1190,15 +1257,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G6" s="25">
+        <v>44473</v>
+      </c>
       <c r="H6" s="9">
         <v>1</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>40</v>
       </c>
@@ -1212,15 +1283,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G7" s="25">
+        <v>44473</v>
+      </c>
       <c r="H7" s="9">
         <v>1</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>25</v>
       </c>
@@ -1234,15 +1309,19 @@
         <v>1</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G8" s="25">
+        <v>44473</v>
+      </c>
       <c r="H8" s="9">
         <v>1</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
@@ -1256,15 +1335,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G9" s="25">
+        <v>44473</v>
+      </c>
       <c r="H9" s="9">
         <v>1</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" spans="1:10" ht="44" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" ht="43.95" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
         <v>41</v>
       </c>
@@ -1278,22 +1361,30 @@
         <v>1</v>
       </c>
       <c r="E10" s="8"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="9"/>
+      <c r="F10" s="25">
+        <v>44482</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="24">
         <v>44471</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="25">
+        <v>44482</v>
+      </c>
       <c r="D11" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>23</v>
@@ -1301,16 +1392,18 @@
       <c r="F11" s="24">
         <v>44473</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H11" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1429,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="21" t="s">
         <v>28</v>
       </c>
@@ -1362,36 +1455,44 @@
       <c r="I13" s="8"/>
       <c r="J13" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="25">
+        <v>44482</v>
+      </c>
+      <c r="C14" s="25">
+        <v>44482</v>
+      </c>
       <c r="D14" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="25">
         <v>44482</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="25">
+        <v>44482</v>
+      </c>
       <c r="H14" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="10"/>
     </row>
-    <row r="15" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="24">
         <v>44471</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="25">
+        <v>44482</v>
+      </c>
       <c r="D15" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>23</v>
@@ -1399,16 +1500,18 @@
       <c r="F15" s="24">
         <v>44473</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H15" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="10"/>
     </row>
-    <row r="16" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>27</v>
       </c>
@@ -1434,27 +1537,33 @@
       <c r="I16" s="8"/>
       <c r="J16" s="10"/>
     </row>
-    <row r="17" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="B17" s="25">
+        <v>44482</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="25">
         <v>44482</v>
       </c>
-      <c r="G17" s="25"/>
+      <c r="G17" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H17" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="10"/>
     </row>
-    <row r="18" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
@@ -1470,13 +1579,21 @@
       <c r="E18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
+      <c r="F18" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="J18" s="10"/>
     </row>
-    <row r="19" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>29</v>
       </c>
@@ -1490,13 +1607,19 @@
         <v>1</v>
       </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="9"/>
+      <c r="F19" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G19" s="25">
+        <v>44473</v>
+      </c>
+      <c r="H19" s="9">
+        <v>1</v>
+      </c>
       <c r="I19" s="8"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
@@ -1510,13 +1633,19 @@
         <v>1</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="9"/>
+      <c r="F20" s="25">
+        <v>44473</v>
+      </c>
+      <c r="G20" s="25">
+        <v>44473</v>
+      </c>
+      <c r="H20" s="9">
+        <v>1</v>
+      </c>
       <c r="I20" s="8"/>
       <c r="J20" s="10"/>
     </row>
-    <row r="21" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
@@ -1530,13 +1659,19 @@
         <v>1</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="9"/>
+      <c r="F21" s="25">
+        <v>44482</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
       <c r="I21" s="8"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
@@ -1552,15 +1687,21 @@
       <c r="E22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="9"/>
+      <c r="F22" s="25">
+        <v>44477</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1</v>
+      </c>
       <c r="I22" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="21" t="s">
         <v>31</v>
       </c>
@@ -1574,15 +1715,19 @@
         <v>1</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="F23" s="25">
+        <v>44477</v>
+      </c>
+      <c r="G23" s="25">
+        <v>44477</v>
+      </c>
       <c r="H23" s="9">
         <v>1</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="21" t="s">
         <v>32</v>
       </c>
@@ -1596,15 +1741,19 @@
         <v>1</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="F24" s="25">
+        <v>44477</v>
+      </c>
+      <c r="G24" s="25">
+        <v>44477</v>
+      </c>
       <c r="H24" s="9">
         <v>1</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="10"/>
     </row>
-    <row r="25" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="21" t="s">
         <v>41</v>
       </c>
@@ -1618,13 +1767,19 @@
         <v>1</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="9"/>
+      <c r="F25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H25" s="9">
+        <v>1</v>
+      </c>
       <c r="I25" s="8"/>
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
@@ -1635,24 +1790,26 @@
         <v>44477</v>
       </c>
       <c r="D26" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="25">
         <v>44478</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="26">
-        <v>0.67</v>
+      <c r="G26" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="9">
+        <v>1</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="21" t="s">
         <v>27</v>
       </c>
@@ -1672,57 +1829,69 @@
       <c r="G27" s="25">
         <v>44478</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="9">
         <v>1</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="25">
+        <v>44482</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D28" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="25">
         <v>44482</v>
       </c>
-      <c r="G28" s="7"/>
+      <c r="G28" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="H28" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="24">
         <v>44474</v>
       </c>
-      <c r="C29" s="24">
-        <v>44481</v>
+      <c r="C29" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="D29" s="9">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="9"/>
+      <c r="F29" s="24">
+        <v>44478</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="9">
+        <v>1</v>
+      </c>
       <c r="I29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J29" s="10"/>
     </row>
-    <row r="30" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="21" t="s">
         <v>33</v>
       </c>
@@ -1736,15 +1905,19 @@
         <v>1</v>
       </c>
       <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
+      <c r="F30" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G30" s="25">
+        <v>44478</v>
+      </c>
       <c r="H30" s="9">
         <v>1</v>
       </c>
       <c r="I30" s="8"/>
       <c r="J30" s="10"/>
     </row>
-    <row r="31" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="21" t="s">
         <v>15</v>
       </c>
@@ -1758,15 +1931,19 @@
         <v>1</v>
       </c>
       <c r="E31" s="8"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="F31" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G31" s="25">
+        <v>44478</v>
+      </c>
       <c r="H31" s="9">
         <v>1</v>
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="10"/>
     </row>
-    <row r="32" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="21" t="s">
         <v>41</v>
       </c>
@@ -1777,25 +1954,33 @@
         <v>44481</v>
       </c>
       <c r="D32" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="8"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="9"/>
+      <c r="F32" s="25">
+        <v>44482</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="9">
+        <v>1</v>
+      </c>
       <c r="I32" s="8"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="24">
         <v>44474</v>
       </c>
-      <c r="C33" s="25"/>
+      <c r="C33" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D33" s="9">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>23</v>
@@ -1803,16 +1988,18 @@
       <c r="F33" s="24">
         <v>44478</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="26">
-        <v>0.8</v>
+      <c r="G33" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="9">
+        <v>1</v>
       </c>
       <c r="I33" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21" t="s">
         <v>27</v>
       </c>
@@ -1838,36 +2025,44 @@
       <c r="I34" s="8"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="B35" s="25">
+        <v>44481</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D35" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="25">
         <v>44482</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="9">
-        <v>0.8</v>
+      <c r="G35" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" s="26">
+        <v>1</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="24">
         <v>44474</v>
       </c>
-      <c r="C36" s="25"/>
+      <c r="C36" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D36" s="9">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>23</v>
@@ -1875,16 +2070,18 @@
       <c r="F36" s="24">
         <v>44478</v>
       </c>
-      <c r="G36" s="25"/>
+      <c r="G36" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="H36" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="21" t="s">
         <v>27</v>
       </c>
@@ -1910,27 +2107,33 @@
       <c r="I37" s="8"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="25">
+        <v>44482</v>
+      </c>
+      <c r="C38" s="25">
+        <v>44482</v>
+      </c>
       <c r="D38" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="25">
         <v>44482</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="9">
-        <v>0.8</v>
+      <c r="G38" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="26">
+        <v>1</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>18</v>
       </c>
@@ -1941,20 +2144,26 @@
         <v>44481</v>
       </c>
       <c r="D39" s="9">
-        <v>0.67</v>
+        <v>1</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="9"/>
+      <c r="F39" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="26">
+        <v>1</v>
+      </c>
       <c r="I39" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="21" t="s">
         <v>34</v>
       </c>
@@ -1968,15 +2177,19 @@
         <v>1</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="9">
+      <c r="F40" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G40" s="25">
+        <v>44478</v>
+      </c>
+      <c r="H40" s="26">
         <v>1</v>
       </c>
       <c r="I40" s="8"/>
       <c r="J40" s="10"/>
     </row>
-    <row r="41" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
         <v>10</v>
       </c>
@@ -1990,15 +2203,19 @@
         <v>1</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="9">
+      <c r="F41" s="25">
+        <v>44478</v>
+      </c>
+      <c r="G41" s="25">
+        <v>44478</v>
+      </c>
+      <c r="H41" s="26">
         <v>1</v>
       </c>
       <c r="I41" s="8"/>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="21" t="s">
         <v>41</v>
       </c>
@@ -2009,25 +2226,33 @@
         <v>44481</v>
       </c>
       <c r="D42" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="9"/>
+      <c r="F42" s="25">
+        <v>44481</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="26">
+        <v>1</v>
+      </c>
       <c r="I42" s="8"/>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="24">
         <v>44474</v>
       </c>
-      <c r="C43" s="25"/>
+      <c r="C43" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D43" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>23</v>
@@ -2035,16 +2260,18 @@
       <c r="F43" s="24">
         <v>44478</v>
       </c>
-      <c r="G43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="H43" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J43" s="10"/>
     </row>
-    <row r="44" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
         <v>36</v>
       </c>
@@ -2070,7 +2297,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="10"/>
     </row>
-    <row r="45" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>31</v>
       </c>
@@ -2096,7 +2323,7 @@
       <c r="I45" s="8"/>
       <c r="J45" s="10"/>
     </row>
-    <row r="46" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>38</v>
       </c>
@@ -2122,7 +2349,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="10"/>
     </row>
-    <row r="47" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="22" t="s">
         <v>37</v>
       </c>
@@ -2148,27 +2375,33 @@
       <c r="I47" s="8"/>
       <c r="J47" s="10"/>
     </row>
-    <row r="48" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
+      <c r="B48" s="25">
+        <v>44482</v>
+      </c>
+      <c r="C48" s="25">
+        <v>44482</v>
+      </c>
       <c r="D48" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="25">
         <v>44482</v>
       </c>
-      <c r="G48" s="25"/>
+      <c r="G48" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="H48" s="26">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I48" s="8"/>
       <c r="J48" s="10"/>
     </row>
-    <row r="49" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>35</v>
       </c>
@@ -2198,1140 +2431,1060 @@
       </c>
       <c r="J49" s="10"/>
     </row>
-    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1013" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1014" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1015" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1016" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="H11:H16 H18:H20 H22 H29">
-    <cfRule type="cellIs" dxfId="33" priority="58" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="cellIs" dxfId="32" priority="57" operator="greaterThan">
+  <conditionalFormatting sqref="H12:H13 H16:H22">
+    <cfRule type="cellIs" dxfId="38" priority="63" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="31" priority="53" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="cellIs" dxfId="30" priority="49" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="cellIs" dxfId="29" priority="47" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="cellIs" dxfId="28" priority="45" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="cellIs" dxfId="27" priority="41" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="26" priority="39" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H38">
-    <cfRule type="cellIs" dxfId="24" priority="31" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="58" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D49">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="H8">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4">
+  <conditionalFormatting sqref="H9">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThan">
+  <conditionalFormatting sqref="H23">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="H24:H29">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
+  <conditionalFormatting sqref="H31:H33">
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43:H47">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
+  <conditionalFormatting sqref="H34:H49">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H26">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
-      <formula>0.99</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
+  <conditionalFormatting sqref="H4">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
+  <conditionalFormatting sqref="H10">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
+  <conditionalFormatting sqref="H11">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+  <conditionalFormatting sqref="H14">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
+  <conditionalFormatting sqref="H15">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>

</xml_diff>